<commit_message>
circos code pending, all else included
</commit_message>
<xml_diff>
--- a/ClusterSubgenomeWorksheet.xlsx
+++ b/ClusterSubgenomeWorksheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-32540" yWindow="3820" windowWidth="27760" windowHeight="15820" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-28660" yWindow="1900" windowWidth="27760" windowHeight="15820" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ClusterAdjacency.csv" sheetId="1" r:id="rId1"/>
@@ -141,8 +141,50 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -156,15 +198,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="51">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -15805,18 +15889,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="6" max="7" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -15837,8 +15921,14 @@
         <f>SUMIF(D1:D25,"=1",E1:E25)</f>
         <v>1292667525</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1">
+        <v>1292667525</v>
+      </c>
+      <c r="I1">
+        <v>1359610</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -15863,8 +15953,14 @@
         <f>F2+F1</f>
         <v>1998320574</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2">
+        <v>705653049</v>
+      </c>
+      <c r="I2">
+        <v>183312</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -15886,7 +15982,7 @@
         <v>0.64687695348724361</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -15904,7 +16000,7 @@
         <v>114285020</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -15922,7 +16018,7 @@
         <v>108854224</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -15940,7 +16036,7 @@
         <v>68299690</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -15958,7 +16054,7 @@
         <v>56279943</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -15976,7 +16072,7 @@
         <v>85024468</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -15994,7 +16090,7 @@
         <v>2636976</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -16012,7 +16108,7 @@
         <v>23760844</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -16030,7 +16126,7 @@
         <v>156796122</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -16048,7 +16144,7 @@
         <v>9783851</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -16066,7 +16162,7 @@
         <v>6887430</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -16084,7 +16180,7 @@
         <v>14580536</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -16102,7 +16198,7 @@
         <v>26171230</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>16</v>
       </c>

</xml_diff>